<commit_message>
337 - fixes emails in excel files and the related tests
</commit_message>
<xml_diff>
--- a/src/test/resources/test_training_wrong_format_at_line_1.xlsx
+++ b/src/test/resources/test_training_wrong_format_at_line_1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>data</t>
   </si>
@@ -44,7 +44,7 @@
     <t>1111111111 1</t>
   </si>
   <si>
-    <t>nemreg1es@mail.com1</t>
+    <t>nemreg1es1@mail.com</t>
   </si>
   <si>
     <t>Most 1es 2</t>
@@ -56,7 +56,7 @@
     <t>1111111111 2</t>
   </si>
   <si>
-    <t>nemreg1es@mail.com2</t>
+    <t>nemreg1es2@mail.com</t>
   </si>
   <si>
     <t>Most 1es 3</t>
@@ -68,7 +68,7 @@
     <t>1111111111 3</t>
   </si>
   <si>
-    <t>nemreg1es@mail.com3</t>
+    <t>nemreg1es3@mail.com</t>
   </si>
   <si>
     <t>Most 1es 4</t>
@@ -80,9 +80,6 @@
     <t>1111111111 4</t>
   </si>
   <si>
-    <t>1111111114@mail.com</t>
-  </si>
-  <si>
     <t>Most 1es 5</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
   </si>
   <si>
     <t>1111111111 5</t>
-  </si>
-  <si>
-    <t>1111111115@mail.com</t>
   </si>
 </sst>
 </file>
@@ -194,7 +188,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -294,25 +288,19 @@
       <c r="F7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>111115</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>